<commit_message>
work on beeswarm graphic:
</commit_message>
<xml_diff>
--- a/code/data/combine.xlsx
+++ b/code/data/combine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennymd/dev/renee-infographic/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4531E7C8-6BBE-534F-ACC4-5A36B7BE15AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC5D8C-8085-FC42-9901-2B3E27B5C689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{0B250B1D-37AA-0544-8798-52B140837C4B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{0B250B1D-37AA-0544-8798-52B140837C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="composite" sheetId="4" r:id="rId1"/>
@@ -20,14 +20,14 @@
     <sheet name="winning drivers" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">composite!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">composite!$A$1:$G$1</definedName>
     <definedName name="teams_active_years" localSheetId="2">'competing years'!$A$1:$C$24</definedName>
     <definedName name="winners_annual" localSheetId="4">'winning drivers'!$A$1:$C$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId6"/>
-    <pivotCache cacheId="19" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="67">
   <si>
     <t>team</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>z_wins</t>
+  </si>
+  <si>
+    <t>log_winningest</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1010,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F0C0D60-FFDA-7D4D-940E-5A1EEBCAF069}" name="PivotTable4" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F0C0D60-FFDA-7D4D-940E-5A1EEBCAF069}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -1110,7 +1113,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4BAAAEEF-A056-EF49-BFF9-D40D4B0282F6}" name="PivotTable3" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4BAAAEEF-A056-EF49-BFF9-D40D4B0282F6}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0">
@@ -1626,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4DA918-70AB-0C42-ADF6-C18075F11885}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1639,7 +1642,7 @@
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -1661,8 +1664,11 @@
       <c r="G1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1673,11 +1679,11 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D17" si="0">C2/B2</f>
+        <f>C2/B2</f>
         <v>1</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E17" si="1">RANK(D2,D$2:D$17)</f>
+        <f>RANK(D2,D$2:D$17)</f>
         <v>1</v>
       </c>
       <c r="F2">
@@ -1688,8 +1694,12 @@
         <f>(C2-C$22)/C$23</f>
         <v>-0.81946788330104392</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <f>LOG10(D2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1700,23 +1710,27 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f>C3/B3</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
+        <f>RANK(D3,D$2:D$17)</f>
         <v>2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F17" si="2">(B3-B$22)/B$23</f>
+        <f>(B3-B$22)/B$23</f>
         <v>-0.72779515535997041</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G17" si="3">(C3-C$22)/C$23</f>
+        <f>(C3-C$22)/C$23</f>
         <v>0.66485130154612992</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <f t="shared" ref="H3:H17" si="0">LOG10(D3)</f>
+        <v>-0.23408320603336796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1727,23 +1741,27 @@
         <v>4</v>
       </c>
       <c r="D4">
+        <f>C4/B4</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="E4">
+        <f>RANK(D4,D$2:D$17)</f>
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f>(B4-B$22)/B$23</f>
+        <v>-0.56827840897970294</v>
+      </c>
+      <c r="G4">
+        <f>(C4-C$22)/C$23</f>
+        <v>-7.730829087745697E-2</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="0"/>
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
-        <v>-0.56827840897970294</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="3"/>
-        <v>-7.730829087745697E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.57403126772771884</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1754,23 +1772,27 @@
         <v>12</v>
       </c>
       <c r="D5">
+        <f>C5/B5</f>
+        <v>0.22641509433962265</v>
+      </c>
+      <c r="E5">
+        <f>RANK(D5,D$2:D$17)</f>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f>(B5-B$22)/B$23</f>
+        <v>1.4522670451703519</v>
+      </c>
+      <c r="G5">
+        <f>(C5-C$22)/C$23</f>
+        <v>1.9017839555854414</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
-        <v>0.22641509433962265</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>1.4522670451703519</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="3"/>
-        <v>1.9017839555854414</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.64509462355316416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1781,23 +1803,27 @@
         <v>15</v>
       </c>
       <c r="D6">
+        <f>C6/B6</f>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="E6">
+        <f>RANK(D6,D$2:D$17)</f>
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f>(B6-B$22)/B$23</f>
+        <v>2.3561952746585342</v>
+      </c>
+      <c r="G6">
+        <f>(C6-C$22)/C$23</f>
+        <v>2.6439435480090285</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>0.21428571428571427</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>2.3561952746585342</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="3"/>
-        <v>2.6439435480090285</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.66900678095857558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1808,23 +1834,27 @@
         <v>2</v>
       </c>
       <c r="D7">
+        <f>C7/B7</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="E7">
+        <f>RANK(D7,D$2:D$17)</f>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f>(B7-B$22)/B$23</f>
+        <v>-0.78096740415339283</v>
+      </c>
+      <c r="G7">
+        <f>(C7-C$22)/C$23</f>
+        <v>-0.57208135249318159</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>-0.78096740415339283</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="3"/>
-        <v>-0.57208135249318159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.74036268949424389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1835,23 +1865,27 @@
         <v>1</v>
       </c>
       <c r="D8">
+        <f>C8/B8</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E8">
+        <f>RANK(D8,D$2:D$17)</f>
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <f>(B8-B$22)/B$23</f>
+        <v>-1.0468286481205054</v>
+      </c>
+      <c r="G8">
+        <f>(C8-C$22)/C$23</f>
+        <v>-0.81946788330104392</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>-1.0468286481205054</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="3"/>
-        <v>-0.81946788330104392</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.77815125038364363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1862,23 +1896,27 @@
         <v>7</v>
       </c>
       <c r="D9">
+        <f>C9/B9</f>
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="E9">
+        <f>RANK(D9,D$2:D$17)</f>
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <f>(B9-B$22)/B$23</f>
+        <v>1.0268890548229719</v>
+      </c>
+      <c r="G9">
+        <f>(C9-C$22)/C$23</f>
+        <v>0.66485130154612992</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
-        <v>0.15555555555555556</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>1.0268890548229719</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="3"/>
-        <v>0.66485130154612992</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.8081144737610868</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1889,23 +1927,27 @@
         <v>6</v>
       </c>
       <c r="D10">
+        <f>C10/B10</f>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="E10">
+        <f>RANK(D10,D$2:D$17)</f>
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <f>(B10-B$22)/B$23</f>
+        <v>0.92054455723612694</v>
+      </c>
+      <c r="G10">
+        <f>(C10-C$22)/C$23</f>
+        <v>0.41746477073826765</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
-        <v>0.13953488372093023</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>0.92054455723612694</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="3"/>
-        <v>0.41746477073826765</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.8553172051959429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1916,23 +1958,27 @@
         <v>4</v>
       </c>
       <c r="D11">
+        <f>C11/B11</f>
+        <v>0.12903225806451613</v>
+      </c>
+      <c r="E11">
+        <f>RANK(D11,D$2:D$17)</f>
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <f>(B11-B$22)/B$23</f>
+        <v>0.282477571715057</v>
+      </c>
+      <c r="G11">
+        <f>(C11-C$22)/C$23</f>
+        <v>-7.730829087745697E-2</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
-        <v>0.12903225806451613</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>0.282477571715057</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="3"/>
-        <v>-7.730829087745697E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.88930170250631035</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1943,23 +1989,27 @@
         <v>2</v>
       </c>
       <c r="D12">
+        <f>C12/B12</f>
+        <v>0.125</v>
+      </c>
+      <c r="E12">
+        <f>RANK(D12,D$2:D$17)</f>
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <f>(B12-B$22)/B$23</f>
+        <v>-0.51510616018628042</v>
+      </c>
+      <c r="G12">
+        <f>(C12-C$22)/C$23</f>
+        <v>-0.57208135249318159</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>-0.51510616018628042</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="3"/>
-        <v>-0.57208135249318159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.90308998699194354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1970,23 +2020,27 @@
         <v>2</v>
       </c>
       <c r="D13">
+        <f>C13/B13</f>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="E13">
+        <f>RANK(D13,D$2:D$17)</f>
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <f>(B13-B$22)/B$23</f>
+        <v>-0.35558941380601294</v>
+      </c>
+      <c r="G13">
+        <f>(C13-C$22)/C$23</f>
+        <v>-0.57208135249318159</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>0.10526315789473684</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
-        <v>-0.35558941380601294</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="3"/>
-        <v>-0.57208135249318159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-0.97772360528884783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1997,23 +2051,27 @@
         <v>1</v>
       </c>
       <c r="D14">
+        <f>C14/B14</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="E14">
+        <f>RANK(D14,D$2:D$17)</f>
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <f>(B14-B$22)/B$23</f>
+        <v>-0.78096740415339283</v>
+      </c>
+      <c r="G14">
+        <f>(C14-C$22)/C$23</f>
+        <v>-0.81946788330104392</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="2"/>
-        <v>-0.78096740415339283</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="3"/>
-        <v>-0.81946788330104392</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-1.0413926851582249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -2024,23 +2082,27 @@
         <v>2</v>
       </c>
       <c r="D15">
+        <f>C15/B15</f>
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="E15">
+        <f>RANK(D15,D$2:D$17)</f>
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <f>(B15-B$22)/B$23</f>
+        <v>6.9788576541367026E-2</v>
+      </c>
+      <c r="G15">
+        <f>(C15-C$22)/C$23</f>
+        <v>-0.57208135249318159</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="0"/>
-        <v>7.407407407407407E-2</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="2"/>
-        <v>6.9788576541367026E-2</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="3"/>
-        <v>-0.57208135249318159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-1.1303337684950061</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2051,23 +2113,27 @@
         <v>2</v>
       </c>
       <c r="D16">
+        <f>C16/B16</f>
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="E16">
+        <f>RANK(D16,D$2:D$17)</f>
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <f>(B16-B$22)/B$23</f>
+        <v>0.176133074128212</v>
+      </c>
+      <c r="G16">
+        <f>(C16-C$22)/C$23</f>
+        <v>-0.57208135249318159</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="0"/>
-        <v>6.8965517241379309E-2</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
-        <v>0.176133074128212</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="3"/>
-        <v>-0.57208135249318159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-1.1613680022349748</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2078,23 +2144,27 @@
         <v>1</v>
       </c>
       <c r="D17">
+        <f>C17/B17</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="E17">
+        <f>RANK(D17,D$2:D$17)</f>
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <f>(B17-B$22)/B$23</f>
+        <v>-0.19607266742574544</v>
+      </c>
+      <c r="G17">
+        <f>(C17-C$22)/C$23</f>
+        <v>-0.81946788330104392</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="0"/>
-        <v>4.5454545454545456E-2</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="2"/>
-        <v>-0.19607266742574544</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="3"/>
-        <v>-0.81946788330104392</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-1.3424226808222062</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22">
         <f>AVERAGE(B2:B17)</f>
         <v>25.6875</v>
@@ -2104,7 +2174,7 @@
         <v>4.3125</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23">
         <f>STDEV(B2:B17)</f>
         <v>18.806802847196899</v>
@@ -2115,8 +2185,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{31493E49-2CDB-754E-AFE1-8C1D44FCB9B4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">
+  <autoFilter ref="A1:G1" xr:uid="{10F88107-D4C1-584D-B4D9-0E073F56CB5E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
       <sortCondition ref="E1:E17"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
save progress on things
</commit_message>
<xml_diff>
--- a/code/data/combine.xlsx
+++ b/code/data/combine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennymd/dev/renee-infographic/code/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennymd/dev/f1-infographic/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC5D8C-8085-FC42-9901-2B3E27B5C689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D28D55A-5C5D-194F-9A3C-E6DF5190DA92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{0B250B1D-37AA-0544-8798-52B140837C4B}"/>
+    <workbookView xWindow="6400" yWindow="3260" windowWidth="25600" windowHeight="15540" xr2:uid="{0B250B1D-37AA-0544-8798-52B140837C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="composite" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="winning drivers" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">composite!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">composite!$A$1:$I$1</definedName>
     <definedName name="teams_active_years" localSheetId="2">'competing years'!$A$1:$C$24</definedName>
     <definedName name="winners_annual" localSheetId="4">'winning drivers'!$A$1:$C$70</definedName>
   </definedNames>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="73">
   <si>
     <t>team</t>
   </si>
@@ -268,6 +268,24 @@
   </si>
   <si>
     <t>log_winningest</t>
+  </si>
+  <si>
+    <t>min opacity</t>
+  </si>
+  <si>
+    <t>max opacity</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>number of pieces</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>opacity step</t>
   </si>
 </sst>
 </file>
@@ -1629,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4DA918-70AB-0C42-ADF6-C18075F11885}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1640,9 +1658,11 @@
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -1667,8 +1687,11 @@
       <c r="H1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1698,8 +1721,11 @@
         <f>LOG10(D2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1726,11 +1752,14 @@
         <v>0.66485130154612992</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H17" si="0">LOG10(D3)</f>
+        <f>LOG10(D3)</f>
         <v>-0.23408320603336796</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1757,11 +1786,14 @@
         <v>-7.730829087745697E-2</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f>LOG10(D4)</f>
         <v>-0.57403126772771884</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1788,11 +1820,14 @@
         <v>1.9017839555854414</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f>LOG10(D5)</f>
         <v>-0.64509462355316416</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1819,11 +1854,14 @@
         <v>2.6439435480090285</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>LOG10(D6)</f>
         <v>-0.66900678095857558</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1850,11 +1888,14 @@
         <v>-0.57208135249318159</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f>LOG10(D7)</f>
         <v>-0.74036268949424389</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1881,11 +1922,14 @@
         <v>-0.81946788330104392</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f>LOG10(D8)</f>
         <v>-0.77815125038364363</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1912,11 +1956,14 @@
         <v>0.66485130154612992</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f>LOG10(D9)</f>
         <v>-0.8081144737610868</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1943,11 +1990,14 @@
         <v>0.41746477073826765</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f>LOG10(D10)</f>
         <v>-0.8553172051959429</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1974,11 +2024,14 @@
         <v>-7.730829087745697E-2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f>LOG10(D11)</f>
         <v>-0.88930170250631035</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2005,11 +2058,14 @@
         <v>-0.57208135249318159</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f>LOG10(D12)</f>
         <v>-0.90308998699194354</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -2036,11 +2092,14 @@
         <v>-0.57208135249318159</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f>LOG10(D13)</f>
         <v>-0.97772360528884783</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -2067,11 +2126,14 @@
         <v>-0.81946788330104392</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f>LOG10(D14)</f>
         <v>-1.0413926851582249</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -2098,11 +2160,14 @@
         <v>-0.57208135249318159</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f>LOG10(D15)</f>
         <v>-1.1303337684950061</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2129,11 +2194,14 @@
         <v>-0.57208135249318159</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f>LOG10(D16)</f>
         <v>-1.1613680022349748</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2160,11 +2228,14 @@
         <v>-0.81946788330104392</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f>LOG10(D17)</f>
         <v>-1.3424226808222062</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22">
         <f>AVERAGE(B2:B17)</f>
         <v>25.6875</v>
@@ -2174,7 +2245,7 @@
         <v>4.3125</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23">
         <f>STDEV(B2:B17)</f>
         <v>18.806802847196899</v>
@@ -2184,10 +2255,52 @@
         <v>4.0422572592550319</v>
       </c>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28">
+        <f>C27-C26</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30">
+        <f>C28/7</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{10F88107-D4C1-584D-B4D9-0E073F56CB5E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
-      <sortCondition ref="E1:E17"/>
+  <autoFilter ref="A1:I1" xr:uid="{DAC93B0D-F48A-EC4A-87E1-7E8F77943D90}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I17">
+      <sortCondition descending="1" ref="D1:D17"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">

</xml_diff>

<commit_message>
work on data more, get to annotating the damn scatter plot
</commit_message>
<xml_diff>
--- a/code/data/combine.xlsx
+++ b/code/data/combine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennymd/dev/f1-infographic/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D28D55A-5C5D-194F-9A3C-E6DF5190DA92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BBCBC1-B6D7-5A44-A16B-20FCE608D206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="3260" windowWidth="25600" windowHeight="15540" xr2:uid="{0B250B1D-37AA-0544-8798-52B140837C4B}"/>
+    <workbookView xWindow="1760" yWindow="5620" windowWidth="25600" windowHeight="15540" xr2:uid="{0B250B1D-37AA-0544-8798-52B140837C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="composite" sheetId="4" r:id="rId1"/>
@@ -1650,7 +1650,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1702,23 +1702,23 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f>C2/B2</f>
+        <f t="shared" ref="D2:D17" si="0">C2/B2</f>
         <v>1</v>
       </c>
       <c r="E2">
-        <f>RANK(D2,D$2:D$17)</f>
+        <f t="shared" ref="E2:E17" si="1">RANK(D2,D$2:D$17)</f>
         <v>1</v>
       </c>
       <c r="F2">
-        <f>(B2-B$22)/B$23</f>
+        <f t="shared" ref="F2:F17" si="2">(B2-B$22)/B$23</f>
         <v>-1.3126898920876178</v>
       </c>
       <c r="G2">
-        <f>(C2-C$22)/C$23</f>
+        <f t="shared" ref="G2:G17" si="3">(C2-C$22)/C$23</f>
         <v>-0.81946788330104392</v>
       </c>
       <c r="H2">
-        <f>LOG10(D2)</f>
+        <f t="shared" ref="H2:H17" si="4">LOG10(D2)</f>
         <v>0</v>
       </c>
       <c r="I2">
@@ -1736,23 +1736,23 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <f>C3/B3</f>
+        <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
       <c r="E3">
-        <f>RANK(D3,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F3">
-        <f>(B3-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>-0.72779515535997041</v>
       </c>
       <c r="G3">
-        <f>(C3-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.66485130154612992</v>
       </c>
       <c r="H3">
-        <f>LOG10(D3)</f>
+        <f t="shared" si="4"/>
         <v>-0.23408320603336796</v>
       </c>
       <c r="I3">
@@ -1770,23 +1770,23 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <f>C4/B4</f>
+        <f t="shared" si="0"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="E4">
-        <f>RANK(D4,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="F4">
-        <f>(B4-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>-0.56827840897970294</v>
       </c>
       <c r="G4">
-        <f>(C4-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-7.730829087745697E-2</v>
       </c>
       <c r="H4">
-        <f>LOG10(D4)</f>
+        <f t="shared" si="4"/>
         <v>-0.57403126772771884</v>
       </c>
       <c r="I4">
@@ -1804,23 +1804,23 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <f>C5/B5</f>
+        <f t="shared" si="0"/>
         <v>0.22641509433962265</v>
       </c>
       <c r="E5">
-        <f>RANK(D5,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F5">
-        <f>(B5-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>1.4522670451703519</v>
       </c>
       <c r="G5">
-        <f>(C5-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>1.9017839555854414</v>
       </c>
       <c r="H5">
-        <f>LOG10(D5)</f>
+        <f t="shared" si="4"/>
         <v>-0.64509462355316416</v>
       </c>
       <c r="I5">
@@ -1838,23 +1838,23 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <f>C6/B6</f>
+        <f t="shared" si="0"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="E6">
-        <f>RANK(D6,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F6">
-        <f>(B6-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>2.3561952746585342</v>
       </c>
       <c r="G6">
-        <f>(C6-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>2.6439435480090285</v>
       </c>
       <c r="H6">
-        <f>LOG10(D6)</f>
+        <f t="shared" si="4"/>
         <v>-0.66900678095857558</v>
       </c>
       <c r="I6">
@@ -1872,23 +1872,23 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <f>C7/B7</f>
+        <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="E7">
-        <f>RANK(D7,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F7">
-        <f>(B7-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>-0.78096740415339283</v>
       </c>
       <c r="G7">
-        <f>(C7-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-0.57208135249318159</v>
       </c>
       <c r="H7">
-        <f>LOG10(D7)</f>
+        <f t="shared" si="4"/>
         <v>-0.74036268949424389</v>
       </c>
       <c r="I7">
@@ -1906,23 +1906,23 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <f>C8/B8</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E8">
-        <f>RANK(D8,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F8">
-        <f>(B8-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>-1.0468286481205054</v>
       </c>
       <c r="G8">
-        <f>(C8-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-0.81946788330104392</v>
       </c>
       <c r="H8">
-        <f>LOG10(D8)</f>
+        <f t="shared" si="4"/>
         <v>-0.77815125038364363</v>
       </c>
       <c r="I8">
@@ -1940,23 +1940,23 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <f>C9/B9</f>
+        <f t="shared" si="0"/>
         <v>0.15555555555555556</v>
       </c>
       <c r="E9">
-        <f>RANK(D9,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F9">
-        <f>(B9-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>1.0268890548229719</v>
       </c>
       <c r="G9">
-        <f>(C9-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.66485130154612992</v>
       </c>
       <c r="H9">
-        <f>LOG10(D9)</f>
+        <f t="shared" si="4"/>
         <v>-0.8081144737610868</v>
       </c>
       <c r="I9">
@@ -1974,23 +1974,23 @@
         <v>6</v>
       </c>
       <c r="D10">
-        <f>C10/B10</f>
+        <f t="shared" si="0"/>
         <v>0.13953488372093023</v>
       </c>
       <c r="E10">
-        <f>RANK(D10,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F10">
-        <f>(B10-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>0.92054455723612694</v>
       </c>
       <c r="G10">
-        <f>(C10-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.41746477073826765</v>
       </c>
       <c r="H10">
-        <f>LOG10(D10)</f>
+        <f t="shared" si="4"/>
         <v>-0.8553172051959429</v>
       </c>
       <c r="I10">
@@ -2008,23 +2008,23 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <f>C11/B11</f>
+        <f t="shared" si="0"/>
         <v>0.12903225806451613</v>
       </c>
       <c r="E11">
-        <f>RANK(D11,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F11">
-        <f>(B11-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>0.282477571715057</v>
       </c>
       <c r="G11">
-        <f>(C11-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-7.730829087745697E-2</v>
       </c>
       <c r="H11">
-        <f>LOG10(D11)</f>
+        <f t="shared" si="4"/>
         <v>-0.88930170250631035</v>
       </c>
       <c r="I11">
@@ -2042,23 +2042,23 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <f>C12/B12</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="E12">
-        <f>RANK(D12,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F12">
-        <f>(B12-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>-0.51510616018628042</v>
       </c>
       <c r="G12">
-        <f>(C12-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-0.57208135249318159</v>
       </c>
       <c r="H12">
-        <f>LOG10(D12)</f>
+        <f t="shared" si="4"/>
         <v>-0.90308998699194354</v>
       </c>
       <c r="I12">
@@ -2076,23 +2076,23 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <f>C13/B13</f>
+        <f t="shared" si="0"/>
         <v>0.10526315789473684</v>
       </c>
       <c r="E13">
-        <f>RANK(D13,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="F13">
-        <f>(B13-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>-0.35558941380601294</v>
       </c>
       <c r="G13">
-        <f>(C13-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-0.57208135249318159</v>
       </c>
       <c r="H13">
-        <f>LOG10(D13)</f>
+        <f t="shared" si="4"/>
         <v>-0.97772360528884783</v>
       </c>
       <c r="I13">
@@ -2110,23 +2110,23 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <f>C14/B14</f>
+        <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="E14">
-        <f>RANK(D14,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="F14">
-        <f>(B14-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>-0.78096740415339283</v>
       </c>
       <c r="G14">
-        <f>(C14-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-0.81946788330104392</v>
       </c>
       <c r="H14">
-        <f>LOG10(D14)</f>
+        <f t="shared" si="4"/>
         <v>-1.0413926851582249</v>
       </c>
       <c r="I14">
@@ -2144,23 +2144,23 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <f>C15/B15</f>
+        <f t="shared" si="0"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="E15">
-        <f>RANK(D15,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="F15">
-        <f>(B15-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>6.9788576541367026E-2</v>
       </c>
       <c r="G15">
-        <f>(C15-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-0.57208135249318159</v>
       </c>
       <c r="H15">
-        <f>LOG10(D15)</f>
+        <f t="shared" si="4"/>
         <v>-1.1303337684950061</v>
       </c>
       <c r="I15">
@@ -2178,23 +2178,23 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <f>C16/B16</f>
+        <f t="shared" si="0"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="E16">
-        <f>RANK(D16,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="F16">
-        <f>(B16-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>0.176133074128212</v>
       </c>
       <c r="G16">
-        <f>(C16-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-0.57208135249318159</v>
       </c>
       <c r="H16">
-        <f>LOG10(D16)</f>
+        <f t="shared" si="4"/>
         <v>-1.1613680022349748</v>
       </c>
       <c r="I16">
@@ -2212,23 +2212,23 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <f>C17/B17</f>
+        <f t="shared" si="0"/>
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="E17">
-        <f>RANK(D17,D$2:D$17)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F17">
-        <f>(B17-B$22)/B$23</f>
+        <f t="shared" si="2"/>
         <v>-0.19607266742574544</v>
       </c>
       <c r="G17">
-        <f>(C17-C$22)/C$23</f>
+        <f t="shared" si="3"/>
         <v>-0.81946788330104392</v>
       </c>
       <c r="H17">
-        <f>LOG10(D17)</f>
+        <f t="shared" si="4"/>
         <v>-1.3424226808222062</v>
       </c>
       <c r="I17">

</xml_diff>